<commit_message>
Melhorias para deixar a lógica de PDFs selecionáveis e PDFs imagens mais próxima, tentando unificar códigos existentes nos 2 casos.
</commit_message>
<xml_diff>
--- a/dados_nfs.xlsx
+++ b/dados_nfs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>Valor NF</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Nome do Arquivo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,8 +486,15 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>250</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025.05.26_PLUXEE BENEF_4992069.pdf</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -508,8 +520,15 @@
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>2000</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.000,00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>COMPRA CREDITO VR FLEX _35826113- NF 04981167.pdf</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -543,8 +562,15 @@
           <t>4500012205</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>1240</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.240,00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>L A SANTANA NFSe 210.pdf</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -578,8 +604,15 @@
           <t>4500012204</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>100</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>100,00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>L A SANTANA NFSe 211.pdf</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -613,8 +646,15 @@
           <t>4500012178</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>21417.2</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>21.417,20</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NF 13788 - CASA BAHIA COMERCIAL LTDA.pdf</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -644,8 +684,15 @@
           <t>4500012187</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>691.83</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>691,83</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NF 158707.pdf</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -679,8 +726,15 @@
           <t>4500012048</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>1750</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1.750,00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NF 1634.pdf</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -714,8 +768,15 @@
           <t>4500012447</t>
         </is>
       </c>
-      <c r="G9" t="n">
-        <v>12753.45</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>12.753,45</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NF 303910.pdf</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -749,8 +810,15 @@
           <t>4500012447</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>12371.95</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>12.371,95</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NF 303911.pdf</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -776,8 +844,15 @@
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
-        <v>5000</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>5.000,00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>NF 7060.pdf</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -811,8 +886,15 @@
           <t>4500012390</t>
         </is>
       </c>
-      <c r="G12" t="n">
-        <v>645.95</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>645,95</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NF 86746 2A SISTEMA AMBIENTAL LTDA.pdf</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -846,8 +928,15 @@
           <t>4500012447</t>
         </is>
       </c>
-      <c r="G13" t="n">
-        <v>12371.95</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>12.371,95</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-303911-boleto.pdf</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -873,8 +962,15 @@
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="n">
-        <v>13564.38</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>13.564,38</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-AAEIFS.pdf</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -900,8 +996,15 @@
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="n">
-        <v>1197.7</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1.197,70</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-AAKCID.pdf</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -931,8 +1034,15 @@
           <t>4500012187</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>691.83</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>691,83</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo.pdf</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -962,8 +1072,15 @@
           <t>4500012186</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>9561.450000000001</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>9.561,45</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NF-e 158706.pdf</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -997,8 +1114,15 @@
           <t>4200002078</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>6630.98</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>6.630,98</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>NF820 CASAS BAHIA R$6.630,98.pdf</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1032,8 +1156,15 @@
           <t>4200001993</t>
         </is>
       </c>
-      <c r="G19" t="n">
-        <v>2250</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2.250,00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NF823 CASAS BAHIA R$2.250,00.pdf</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1067,8 +1198,15 @@
           <t>4500011953</t>
         </is>
       </c>
-      <c r="G20" t="n">
-        <v>600.02</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>600,02</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>NFSe22340_40712883000187.pdf</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1098,8 +1236,15 @@
           <t>4500012841</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>5000</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>5.000,00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>NFSe3765_02878522000116.pdf</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1133,8 +1278,15 @@
           <t>4500012242</t>
         </is>
       </c>
-      <c r="G22" t="n">
-        <v>27533.95</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>27.533,95</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>NFSe5661_03558771000197.pdf</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1168,8 +1320,15 @@
           <t>4500011934</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>1161.94</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1.161,94</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>NFSe_411_ICONREALTY_PLFALESIM.pdf</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1203,8 +1362,15 @@
           <t>4500012080</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>300</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>300,00</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nota 2422.pdf</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1238,8 +1404,15 @@
           <t>4500012252</t>
         </is>
       </c>
-      <c r="G25" t="n">
-        <v>5600</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>5.600,00</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>nota_329557 (NFSe).pdf</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1273,8 +1446,15 @@
           <t>4500012252</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>5600</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>5.600,00</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>nota_336834 (NFSe).pdf</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1308,8 +1488,15 @@
           <t>4500012192</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>15000</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>15.000,00</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>N_2025.05.26_000_7507_4500012192.pdf</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1343,8 +1530,15 @@
           <t>4500012306</t>
         </is>
       </c>
-      <c r="G28" t="n">
-        <v>254</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>254,00</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_000_10792_4500012306.pdf</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1378,8 +1572,15 @@
           <t>4500012330</t>
         </is>
       </c>
-      <c r="G29" t="n">
-        <v>234</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>234,00</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_000_10802_4500012330.pdf</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1413,8 +1614,15 @@
           <t>4500011946</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>201.25</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>201,25</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_009_40839_4500011946.pdf</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1448,8 +1656,15 @@
           <t>4500012249</t>
         </is>
       </c>
-      <c r="G31" t="n">
-        <v>250</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>RETHA ITAQUERA - NF 25269 - MAIO.pdf</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste da captura de CNPJ
</commit_message>
<xml_diff>
--- a/dados_nfs.xlsx
+++ b/dados_nfs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,39 +464,1370 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>04992069</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>69034668000156</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025.05.26_PLUXEE BENEF_4992069.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>04981167</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>30/04/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>69034668000156</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.000,00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>COMPRA CREDITO VR FLEX _35826113- NF 04981167.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>00000210</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>46059301000191</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4700001625</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>4500012205</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.240,00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>L A SANTANA NFSe 210.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>00000211</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>46059301000191</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4700001627</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4500012204</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>100,00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>L A SANTANA NFSe 211.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>00013788</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>01/05/2025</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11.915.135/0001-01</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>59.291.534/0001-67</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>03871618000115</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4700000295</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4500012178</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>21.417,20</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>NF 13788 - CASA BAHIA COMERCIAL LTDA.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>00158707</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>00910509000414</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4500012187</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>691,83</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NF 158707.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>00001634</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>03519943000113</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4700001150</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>4500012048</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1.750,00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NF 1634.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>00303910</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>07073027001982</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4700000179</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>4500012447</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>12.753,45</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NF 303910.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>00303911</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>07073027001982</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4700000179</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4500012447</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>12.371,95</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NF 303911.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>00007060</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10597372000109</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>5.000,00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>NF 7060.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>00086746</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11832260000140</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4700001539</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4500012390</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>645,95</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NF 86746 2A SISTEMA AMBIENTAL LTDA.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>00303911</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>07073027001982</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4700000179</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>4500012447</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>12.371,95</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-303911-boleto.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04123511</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>53113791000122</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>13.564,38</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-AAEIFS.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>04123599</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>53113791000122</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1.197,70</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo-AAKCID.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>00159209</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08/05/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>00910509000414</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>4500012187</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>691,83</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NF-e - Nota Fiscal Eletrônica de Serviços - São Paulo.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>00158706</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>00910509000414</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>4500012186</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>9.561,45</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NF-e 158706.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>00000820</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>17381049000134</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4700002634</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>4200002078</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>6.630,98</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>NF820 CASAS BAHIA R$6.630,98.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>00000823</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>08/05/2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>17381049000134</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>4700002349</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>4200001993</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2.250,00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NF823 CASAS BAHIA R$2.250,00.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>00022340</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>40712883000187</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>4700000585</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>4500011953</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>600,02</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>NFSe22340_40712883000187.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>00003765</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>02878522000116</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>19760435000162</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>4500012841</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>5.000,00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>NFSe3765_02878522000116.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>00005661</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>03558771000197</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>4700001935</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>4500012242</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>27.533,95</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>NFSe5661_03558771000197.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>000411</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>50670703000103</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>4800000009</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>4500011934</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1.161,94</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>NFSe_411_ICONREALTY_PLFALESIM.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>011845</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>07/05/2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>08976076000169</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>4500012712</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>75,00</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nota 11845.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>00002422</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>44351601000114</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>13718634000126</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>4700000018</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>4500012080</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>300,00</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nota 2422.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>69865</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>01/05/2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>11915135000101</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>4700001043</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>4500012195</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>707,34</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Nota 69865.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>329557</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>24166595000118</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>4700002146</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>4500012252</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>5.600,00</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>nota_329557 (NFSe).pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>336834</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>10/05/2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>24166595000118</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>4700002146</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>4500012252</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>5.600,00</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>nota_336834 (NFSe).pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0007507</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>19964645000172</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>4700001624</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4500012192</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>15.000,00</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>N_2025.05.26_000_7507_4500012192.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>00098089</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>08689801000118</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>4800000014</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>4500012210</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>336,25</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>N_2025.06.02_000_98089_4500012210.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>00098038</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>08689801000118</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>4800000015</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>4500012244</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>171,13</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>N_2025.06.02_009_98088_4500012244.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>00010792</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>26771739000190</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>4700002490</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>4500012306</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>254,00</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_000_10792_4500012306.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>00010802</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05/05/2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>26771739000190</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>4700002496</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4500012330</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>234,00</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_000_10802_4500012330.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>00040839</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>06/05/2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>02983477000160</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>00278017000105</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>4700001509</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>4500011946</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>201,25</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>N_2025.06.03_009_40839_4500011946.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>00025269</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>68859503000150</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>59291534000167</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>4700002020</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4500012249</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>250,00</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>RETHA ITAQUERA - NF 25269 - MAIO.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Testes e correções do arquivo unificado.
</commit_message>
<xml_diff>
--- a/dados_nfs.xlsx
+++ b/dados_nfs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>69034668000156</t>
+          <t>69.034.668/0001-56</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00278017000105</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -510,12 +510,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>69034668000156</t>
+          <t>69.034.668/0001-56</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -544,12 +544,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>46059301000191</t>
+          <t>46.059.301/0001-91</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -586,12 +586,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>46059301000191</t>
+          <t>46.059.301/0001-91</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00278017000105</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -628,12 +628,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>03871618000115</t>
+          <t>03.871.618/0001-15</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -670,12 +670,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>00910509000414</t>
+          <t>00.910.509/0004-14</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -708,12 +708,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>03519943000113</t>
+          <t>03.519.943/0001-13</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -750,12 +750,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>07073027001982</t>
+          <t>07.073.027/0019-82</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -792,12 +792,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>07073027001982</t>
+          <t>07.073.027/0019-82</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10597372000109</t>
+          <t>10.597.372/0001-09</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00278017000105</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -868,12 +868,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11832260000140</t>
+          <t>11.832.260/0001-40</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -910,12 +910,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>07073027001982</t>
+          <t>07.073.027/0019-82</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -952,12 +952,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>53113791000122</t>
+          <t>53.113.791/0001-22</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -986,12 +986,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>53113791000122</t>
+          <t>53.113.791/0001-22</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1020,12 +1020,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>00910509000414</t>
+          <t>00.910.509/0004-14</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1058,12 +1058,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>00910509000414</t>
+          <t>00.910.509/0004-14</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1096,12 +1096,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17381049000134</t>
+          <t>17.381.049/0001-34</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1138,12 +1138,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17381049000134</t>
+          <t>17.381.049/0001-34</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1180,12 +1180,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>40712883000187</t>
+          <t>40.712.883/0001-87</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>00278017000105</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1222,12 +1222,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>02878522000116</t>
+          <t>02.878.522/0001-16</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>19760435000162</t>
+          <t>19.760.435/0001-62</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1260,12 +1260,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>03558771000197</t>
+          <t>03.558.771/0001-97</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1302,12 +1302,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>50670703000103</t>
+          <t>50.670.703/0001-03</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1344,12 +1344,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>08976076000169</t>
+          <t>08.976.076/0001-69</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1382,12 +1382,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>44351601000114</t>
+          <t>44.351.601/0001-14</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>13718634000126</t>
+          <t>13.718.634/0001-26</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1424,12 +1424,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11915135000101</t>
+          <t>11.915.135/0001-01</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1456,91 +1456,91 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>329557</t>
+          <t>0007507</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>09/04/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>24166595000118</t>
+          <t>19.964.645/0001-72</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4700002146</t>
+          <t>4700001624</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>4500012252</t>
+          <t>4500012192</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>5.600,00</t>
+          <t>15.000,00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>nota_329557 (NFSe).pdf</t>
+          <t>N_2025.05.26_000_7507_4500012192.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>336834</t>
+          <t>00098089</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>10/05/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>24166595000118</t>
+          <t>08.689.801/0001-18</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4700002146</t>
+          <t>4800000014</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>4500012252</t>
+          <t>4500012210</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>5.600,00</t>
+          <t>336,25</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>nota_336834 (NFSe).pdf</t>
+          <t>N_2025.06.02_000_98089_4500012210.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0007507</t>
+          <t>00098038</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1550,282 +1550,198 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>19964645000172</t>
+          <t>08.689.801/0001-18</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4700001624</t>
+          <t>4800000015</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>4500012192</t>
+          <t>4500012244</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>15.000,00</t>
+          <t>171,13</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>N_2025.05.26_000_7507_4500012192.pdf</t>
+          <t>N_2025.06.02_009_98088_4500012244.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>00098089</t>
+          <t>00010792</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>08689801000118</t>
+          <t>26.771.739/0001-90</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4800000014</t>
+          <t>4700002490</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4500012210</t>
+          <t>4500012306</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>336,25</t>
+          <t>254,00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>N_2025.06.02_000_98089_4500012210.pdf</t>
+          <t>N_2025.06.03_000_10792_4500012306.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>00098038</t>
+          <t>00010802</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>08689801000118</t>
+          <t>26.771.739/0001-90</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>00278017000105</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4800000015</t>
+          <t>4700002496</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>4500012244</t>
+          <t>4500012330</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>171,13</t>
+          <t>234,00</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>N_2025.06.02_009_98088_4500012244.pdf</t>
+          <t>N_2025.06.03_000_10802_4500012330.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>00010792</t>
+          <t>00040839</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>06/05/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>26771739000190</t>
+          <t>02.983.477/0001-60</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>00.278.017/0001-05</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4700002490</t>
+          <t>4700001509</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>4500012306</t>
+          <t>4500011946</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>254,00</t>
+          <t>201,25</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>N_2025.06.03_000_10792_4500012306.pdf</t>
+          <t>N_2025.06.03_009_40839_4500011946.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>00010802</t>
+          <t>00025269</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>26771739000190</t>
+          <t>68.859.503/0001-50</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>59291534000167</t>
+          <t>59.291.534/0001-67</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4700002496</t>
+          <t>4700002020</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>4500012330</t>
+          <t>4500012249</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>234,00</t>
+          <t>250,00</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
-        <is>
-          <t>N_2025.06.03_000_10802_4500012330.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>00040839</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>06/05/2025</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>02983477000160</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>00278017000105</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>4700001509</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>4500011946</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>201,25</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>N_2025.06.03_009_40839_4500011946.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>00025269</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>02/05/2025</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>68859503000150</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>59291534000167</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>4700002020</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>4500012249</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>250,00</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
         <is>
           <t>RETHA ITAQUERA - NF 25269 - MAIO.pdf</t>
         </is>

</xml_diff>

<commit_message>
Mais uma atualização de arquivos e inclusão do teste nanonets
</commit_message>
<xml_diff>
--- a/dados_nfs.xlsx
+++ b/dados_nfs.xlsx
@@ -466,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>1268</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -481,19 +481,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>34.499.567/0004-19</t>
+          <t>31.439.951/0003-57</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.331,28</t>
+          <t>582,00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025.05.30_PORTO SEGURO_211356.PDF</t>
+          <t>2025.05.30_PORTO SEGURO_211368.PDF</t>
         </is>
       </c>
     </row>

</xml_diff>